<commit_message>
modify bench result processed file
</commit_message>
<xml_diff>
--- a/bench-results/2020-03-03/bench-result.xlsx
+++ b/bench-results/2020-03-03/bench-result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludovicmouline/Documents/Thesis/DucPropagationJava/bench-results/2020-03-03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{39E3FE71-2B58-8B42-BD4A-4DD568C4E2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{547C83A6-A8B2-EF4E-A0E2-89996AC3B6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="2"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="171">
   <si>
     <t>Benchmark</t>
   </si>
@@ -610,6 +610,15 @@
   </si>
   <si>
     <t>Uncertain  (µs/op)</t>
+  </si>
+  <si>
+    <t>Parallel@Transformer</t>
+  </si>
+  <si>
+    <t>Parallel@Cabinet</t>
+  </si>
+  <si>
+    <t>Indirect Parallel</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1146,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1177,6 +1186,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1379,13 +1389,13 @@
                   <c:v>Cabinet</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ParaTransformer</c:v>
+                  <c:v>Parallel@Transformer</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ParaCabinet</c:v>
+                  <c:v>Parallel@Cabinet</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>IndirectPara</c:v>
+                  <c:v>Indirect Parallel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1463,13 +1473,13 @@
                   <c:v>Cabinet</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ParaTransformer</c:v>
+                  <c:v>Parallel@Transformer</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ParaCabinet</c:v>
+                  <c:v>Parallel@Cabinet</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>IndirectPara</c:v>
+                  <c:v>Indirect Parallel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1773,8 +1783,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15267869572729742"/>
-          <c:y val="0.16781198930322389"/>
+          <c:x val="0.14434925504742263"/>
+          <c:y val="0.15130255534095974"/>
           <c:w val="0.21910813812850197"/>
           <c:h val="0.12945412349772067"/>
         </c:manualLayout>
@@ -3272,8 +3282,8 @@
       <xdr:rowOff>241300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
@@ -6033,10 +6043,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:G9"/>
+  <dimension ref="C4:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R51" sqref="R51"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -6050,7 +6060,7 @@
     <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7">
+    <row r="4" spans="3:9">
       <c r="C4" s="6" t="s">
         <v>158</v>
       </c>
@@ -6066,8 +6076,14 @@
       <c r="G4" s="5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="3:7">
+      <c r="H4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9">
       <c r="C5" s="4" t="s">
         <v>159</v>
       </c>
@@ -6087,8 +6103,16 @@
         <f>E5*1000</f>
         <v>1.5740000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="3:7">
+      <c r="H5" s="4">
+        <f>G5-F5</f>
+        <v>0.66825000000000012</v>
+      </c>
+      <c r="I5" s="9">
+        <f>H5/F5</f>
+        <v>0.73778636489097449</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9">
       <c r="C6" s="4" t="s">
         <v>160</v>
       </c>
@@ -6108,10 +6132,18 @@
         <f t="shared" ref="G6:G9" si="1">E6*1000</f>
         <v>6.8359999999999994</v>
       </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="4" t="s">
-        <v>161</v>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6:H9" si="2">G6-F6</f>
+        <v>1.918333333333333</v>
+      </c>
+      <c r="I6" s="9">
+        <f>H6/F6</f>
+        <v>0.39009015115569712</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9">
+      <c r="C7" s="15" t="s">
+        <v>168</v>
       </c>
       <c r="D7" s="4">
         <f>AVERAGE(ParaTransformer!C4:C20)</f>
@@ -6129,10 +6161,18 @@
         <f t="shared" si="1"/>
         <v>9.596823529411763</v>
       </c>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="4" t="s">
-        <v>162</v>
+      <c r="H7" s="4">
+        <f t="shared" si="2"/>
+        <v>2.5096470588235285</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" ref="I6:I9" si="3">H7/F7</f>
+        <v>0.35411098753340736</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9">
+      <c r="C8" s="15" t="s">
+        <v>169</v>
       </c>
       <c r="D8" s="4">
         <f>AVERAGE(ParaCabinet!C4:C22)</f>
@@ -6150,10 +6190,18 @@
         <f t="shared" si="1"/>
         <v>14.079789473684215</v>
       </c>
-    </row>
-    <row r="9" spans="3:7">
+      <c r="H8" s="4">
+        <f t="shared" si="2"/>
+        <v>3.2437894736842168</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="3"/>
+        <v>0.29935303374715921</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9">
       <c r="C9" s="4" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D9" s="4">
         <f>AVERAGE(IndirectPara!C4:C6)</f>
@@ -6170,6 +6218,14 @@
       <c r="G9" s="4">
         <f t="shared" si="1"/>
         <v>18.225000000000001</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="2"/>
+        <v>3.7916666666666679</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="3"/>
+        <v>0.26270207852194005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>